<commit_message>
Fix Austrian population mortality, fix plotMortalityTables (axes labels not overridable)
</commit_message>
<xml_diff>
--- a/data-raw/Austria/Austria_JaehrlicheSterbetafeln_1947-2022.xlsx
+++ b/data-raw/Austria/Austria_JaehrlicheSterbetafeln_1947-2022.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t xml:space="preserve">Jährliche Sterbetafeln Österreich Männer, 1947-2022</t>
   </si>
@@ -22,7 +22,7 @@
     <t xml:space="preserve">Quelle: Statistik Austria, https://www.statistik.at/statistiken/bevoelkerung-und-soziales/bevoelkerung/demographische-indikatoren-und-tafeln/sterbetafeln</t>
   </si>
   <si>
-    <t xml:space="preserve">row.names</t>
+    <t xml:space="preserve">Alter</t>
   </si>
   <si>
     <t xml:space="preserve">1947</t>
@@ -253,309 +253,6 @@
     <t xml:space="preserve">2022</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">91</t>
-  </si>
-  <si>
-    <t xml:space="preserve">92</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jährliche Sterbetafeln Österreich Frauen, 1947-2022</t>
   </si>
   <si>
@@ -608,7 +305,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A4:BY105" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A4:BY105"/>
   <tableColumns count="77">
-    <tableColumn id="1" name="row.names"/>
+    <tableColumn id="1" name="Alter"/>
     <tableColumn id="2" name="1947"/>
     <tableColumn id="3" name="1948"/>
     <tableColumn id="4" name="1949"/>
@@ -694,7 +391,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:BY105" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A4:BY105"/>
   <tableColumns count="77">
-    <tableColumn id="1" name="row.names"/>
+    <tableColumn id="1" name="Alter"/>
     <tableColumn id="2" name="1947"/>
     <tableColumn id="3" name="1948"/>
     <tableColumn id="4" name="1949"/>
@@ -780,7 +477,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A4:V105" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A4:V105"/>
   <tableColumns count="22">
-    <tableColumn id="1" name="row.names"/>
+    <tableColumn id="1" name="Alter"/>
     <tableColumn id="2" name="2002"/>
     <tableColumn id="3" name="2003"/>
     <tableColumn id="4" name="2004"/>
@@ -1339,8 +1036,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>79</v>
+      <c r="A5" t="n">
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>0.086051</v>
@@ -1572,8 +1269,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>80</v>
+      <c r="A6" t="n">
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>0.008201</v>
@@ -1805,8 +1502,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>81</v>
+      <c r="A7" t="n">
+        <v>2</v>
       </c>
       <c r="B7" t="n">
         <v>0.004932</v>
@@ -2038,8 +1735,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>82</v>
+      <c r="A8" t="n">
+        <v>3</v>
       </c>
       <c r="B8" t="n">
         <v>0.003341</v>
@@ -2271,8 +1968,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>83</v>
+      <c r="A9" t="n">
+        <v>4</v>
       </c>
       <c r="B9" t="n">
         <v>0.00271</v>
@@ -2504,8 +2201,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>84</v>
+      <c r="A10" t="n">
+        <v>5</v>
       </c>
       <c r="B10" t="n">
         <v>0.001983</v>
@@ -2737,8 +2434,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>85</v>
+      <c r="A11" t="n">
+        <v>6</v>
       </c>
       <c r="B11" t="n">
         <v>0.001448</v>
@@ -2970,8 +2667,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>86</v>
+      <c r="A12" t="n">
+        <v>7</v>
       </c>
       <c r="B12" t="n">
         <v>0.001654</v>
@@ -3203,8 +2900,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>87</v>
+      <c r="A13" t="n">
+        <v>8</v>
       </c>
       <c r="B13" t="n">
         <v>0.001486</v>
@@ -3436,8 +3133,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>88</v>
+      <c r="A14" t="n">
+        <v>9</v>
       </c>
       <c r="B14" t="n">
         <v>0.001032</v>
@@ -3669,8 +3366,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>89</v>
+      <c r="A15" t="n">
+        <v>10</v>
       </c>
       <c r="B15" t="n">
         <v>0.001345</v>
@@ -3902,8 +3599,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>90</v>
+      <c r="A16" t="n">
+        <v>11</v>
       </c>
       <c r="B16" t="n">
         <v>0.001628</v>
@@ -4135,8 +3832,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>91</v>
+      <c r="A17" t="n">
+        <v>12</v>
       </c>
       <c r="B17" t="n">
         <v>0.001043</v>
@@ -4368,8 +4065,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>92</v>
+      <c r="A18" t="n">
+        <v>13</v>
       </c>
       <c r="B18" t="n">
         <v>0.001079</v>
@@ -4601,8 +4298,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>93</v>
+      <c r="A19" t="n">
+        <v>14</v>
       </c>
       <c r="B19" t="n">
         <v>0.001449</v>
@@ -4834,8 +4531,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>94</v>
+      <c r="A20" t="n">
+        <v>15</v>
       </c>
       <c r="B20" t="n">
         <v>0.001677</v>
@@ -5067,8 +4764,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>95</v>
+      <c r="A21" t="n">
+        <v>16</v>
       </c>
       <c r="B21" t="n">
         <v>0.001582</v>
@@ -5300,8 +4997,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>96</v>
+      <c r="A22" t="n">
+        <v>17</v>
       </c>
       <c r="B22" t="n">
         <v>0.002314</v>
@@ -5533,8 +5230,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>97</v>
+      <c r="A23" t="n">
+        <v>18</v>
       </c>
       <c r="B23" t="n">
         <v>0.002521</v>
@@ -5766,8 +5463,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>98</v>
+      <c r="A24" t="n">
+        <v>19</v>
       </c>
       <c r="B24" t="n">
         <v>0.003117</v>
@@ -5999,8 +5696,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>99</v>
+      <c r="A25" t="n">
+        <v>20</v>
       </c>
       <c r="B25" t="n">
         <v>0.003236</v>
@@ -6232,8 +5929,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>100</v>
+      <c r="A26" t="n">
+        <v>21</v>
       </c>
       <c r="B26" t="n">
         <v>0.003088</v>
@@ -6465,8 +6162,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>101</v>
+      <c r="A27" t="n">
+        <v>22</v>
       </c>
       <c r="B27" t="n">
         <v>0.003753</v>
@@ -6698,8 +6395,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>102</v>
+      <c r="A28" t="n">
+        <v>23</v>
       </c>
       <c r="B28" t="n">
         <v>0.003816</v>
@@ -6931,8 +6628,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>103</v>
+      <c r="A29" t="n">
+        <v>24</v>
       </c>
       <c r="B29" t="n">
         <v>0.003476</v>
@@ -7164,8 +6861,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>104</v>
+      <c r="A30" t="n">
+        <v>25</v>
       </c>
       <c r="B30" t="n">
         <v>0.0033</v>
@@ -7397,8 +7094,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>105</v>
+      <c r="A31" t="n">
+        <v>26</v>
       </c>
       <c r="B31" t="n">
         <v>0.003272</v>
@@ -7630,8 +7327,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>106</v>
+      <c r="A32" t="n">
+        <v>27</v>
       </c>
       <c r="B32" t="n">
         <v>0.003715</v>
@@ -7863,8 +7560,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>107</v>
+      <c r="A33" t="n">
+        <v>28</v>
       </c>
       <c r="B33" t="n">
         <v>0.003085</v>
@@ -8096,8 +7793,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>108</v>
+      <c r="A34" t="n">
+        <v>29</v>
       </c>
       <c r="B34" t="n">
         <v>0.003056</v>
@@ -8329,8 +8026,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>109</v>
+      <c r="A35" t="n">
+        <v>30</v>
       </c>
       <c r="B35" t="n">
         <v>0.003868</v>
@@ -8562,8 +8259,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>110</v>
+      <c r="A36" t="n">
+        <v>31</v>
       </c>
       <c r="B36" t="n">
         <v>0.003289</v>
@@ -8795,8 +8492,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>111</v>
+      <c r="A37" t="n">
+        <v>32</v>
       </c>
       <c r="B37" t="n">
         <v>0.003879</v>
@@ -9028,8 +8725,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>112</v>
+      <c r="A38" t="n">
+        <v>33</v>
       </c>
       <c r="B38" t="n">
         <v>0.003254</v>
@@ -9261,8 +8958,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>113</v>
+      <c r="A39" t="n">
+        <v>34</v>
       </c>
       <c r="B39" t="n">
         <v>0.00401</v>
@@ -9494,8 +9191,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
-        <v>114</v>
+      <c r="A40" t="n">
+        <v>35</v>
       </c>
       <c r="B40" t="n">
         <v>0.0033</v>
@@ -9727,8 +9424,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>115</v>
+      <c r="A41" t="n">
+        <v>36</v>
       </c>
       <c r="B41" t="n">
         <v>0.004335</v>
@@ -9960,8 +9657,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>116</v>
+      <c r="A42" t="n">
+        <v>37</v>
       </c>
       <c r="B42" t="n">
         <v>0.00439</v>
@@ -10193,8 +9890,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>117</v>
+      <c r="A43" t="n">
+        <v>38</v>
       </c>
       <c r="B43" t="n">
         <v>0.005084</v>
@@ -10426,8 +10123,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>118</v>
+      <c r="A44" t="n">
+        <v>39</v>
       </c>
       <c r="B44" t="n">
         <v>0.004882</v>
@@ -10659,8 +10356,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s">
-        <v>119</v>
+      <c r="A45" t="n">
+        <v>40</v>
       </c>
       <c r="B45" t="n">
         <v>0.005049</v>
@@ -10892,8 +10589,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
-        <v>120</v>
+      <c r="A46" t="n">
+        <v>41</v>
       </c>
       <c r="B46" t="n">
         <v>0.005</v>
@@ -11125,8 +10822,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s">
-        <v>121</v>
+      <c r="A47" t="n">
+        <v>42</v>
       </c>
       <c r="B47" t="n">
         <v>0.005775</v>
@@ -11358,8 +11055,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>122</v>
+      <c r="A48" t="n">
+        <v>43</v>
       </c>
       <c r="B48" t="n">
         <v>0.006038</v>
@@ -11591,8 +11288,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s">
-        <v>123</v>
+      <c r="A49" t="n">
+        <v>44</v>
       </c>
       <c r="B49" t="n">
         <v>0.006369</v>
@@ -11824,8 +11521,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>124</v>
+      <c r="A50" t="n">
+        <v>45</v>
       </c>
       <c r="B50" t="n">
         <v>0.007155</v>
@@ -12057,8 +11754,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s">
-        <v>125</v>
+      <c r="A51" t="n">
+        <v>46</v>
       </c>
       <c r="B51" t="n">
         <v>0.007985</v>
@@ -12290,8 +11987,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>126</v>
+      <c r="A52" t="n">
+        <v>47</v>
       </c>
       <c r="B52" t="n">
         <v>0.008276</v>
@@ -12523,8 +12220,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s">
-        <v>127</v>
+      <c r="A53" t="n">
+        <v>48</v>
       </c>
       <c r="B53" t="n">
         <v>0.009564</v>
@@ -12756,8 +12453,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s">
-        <v>128</v>
+      <c r="A54" t="n">
+        <v>49</v>
       </c>
       <c r="B54" t="n">
         <v>0.009447</v>
@@ -12989,8 +12686,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s">
-        <v>129</v>
+      <c r="A55" t="n">
+        <v>50</v>
       </c>
       <c r="B55" t="n">
         <v>0.011287</v>
@@ -13222,8 +12919,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s">
-        <v>130</v>
+      <c r="A56" t="n">
+        <v>51</v>
       </c>
       <c r="B56" t="n">
         <v>0.011419</v>
@@ -13455,8 +13152,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="s">
-        <v>131</v>
+      <c r="A57" t="n">
+        <v>52</v>
       </c>
       <c r="B57" t="n">
         <v>0.013625</v>
@@ -13688,8 +13385,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s">
-        <v>132</v>
+      <c r="A58" t="n">
+        <v>53</v>
       </c>
       <c r="B58" t="n">
         <v>0.013115</v>
@@ -13921,8 +13618,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s">
-        <v>133</v>
+      <c r="A59" t="n">
+        <v>54</v>
       </c>
       <c r="B59" t="n">
         <v>0.013058</v>
@@ -14154,8 +13851,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s">
-        <v>134</v>
+      <c r="A60" t="n">
+        <v>55</v>
       </c>
       <c r="B60" t="n">
         <v>0.016094</v>
@@ -14387,8 +14084,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s">
-        <v>135</v>
+      <c r="A61" t="n">
+        <v>56</v>
       </c>
       <c r="B61" t="n">
         <v>0.01839</v>
@@ -14620,8 +14317,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
-        <v>136</v>
+      <c r="A62" t="n">
+        <v>57</v>
       </c>
       <c r="B62" t="n">
         <v>0.018256</v>
@@ -14853,8 +14550,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s">
-        <v>137</v>
+      <c r="A63" t="n">
+        <v>58</v>
       </c>
       <c r="B63" t="n">
         <v>0.019049</v>
@@ -15086,8 +14783,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s">
-        <v>138</v>
+      <c r="A64" t="n">
+        <v>59</v>
       </c>
       <c r="B64" t="n">
         <v>0.020729</v>
@@ -15319,8 +15016,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s">
-        <v>139</v>
+      <c r="A65" t="n">
+        <v>60</v>
       </c>
       <c r="B65" t="n">
         <v>0.023206</v>
@@ -15552,8 +15249,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s">
-        <v>140</v>
+      <c r="A66" t="n">
+        <v>61</v>
       </c>
       <c r="B66" t="n">
         <v>0.024779</v>
@@ -15785,8 +15482,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s">
-        <v>141</v>
+      <c r="A67" t="n">
+        <v>62</v>
       </c>
       <c r="B67" t="n">
         <v>0.027189</v>
@@ -16018,8 +15715,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s">
-        <v>142</v>
+      <c r="A68" t="n">
+        <v>63</v>
       </c>
       <c r="B68" t="n">
         <v>0.028431</v>
@@ -16251,8 +15948,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="s">
-        <v>143</v>
+      <c r="A69" t="n">
+        <v>64</v>
       </c>
       <c r="B69" t="n">
         <v>0.032255</v>
@@ -16484,8 +16181,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="s">
-        <v>144</v>
+      <c r="A70" t="n">
+        <v>65</v>
       </c>
       <c r="B70" t="n">
         <v>0.03518</v>
@@ -16717,8 +16414,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="s">
-        <v>145</v>
+      <c r="A71" t="n">
+        <v>66</v>
       </c>
       <c r="B71" t="n">
         <v>0.037686</v>
@@ -16950,8 +16647,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="s">
-        <v>146</v>
+      <c r="A72" t="n">
+        <v>67</v>
       </c>
       <c r="B72" t="n">
         <v>0.039759</v>
@@ -17183,8 +16880,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s">
-        <v>147</v>
+      <c r="A73" t="n">
+        <v>68</v>
       </c>
       <c r="B73" t="n">
         <v>0.046328</v>
@@ -17416,8 +17113,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s">
-        <v>148</v>
+      <c r="A74" t="n">
+        <v>69</v>
       </c>
       <c r="B74" t="n">
         <v>0.050548</v>
@@ -17649,8 +17346,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="s">
-        <v>149</v>
+      <c r="A75" t="n">
+        <v>70</v>
       </c>
       <c r="B75" t="n">
         <v>0.053121</v>
@@ -17882,8 +17579,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="s">
-        <v>150</v>
+      <c r="A76" t="n">
+        <v>71</v>
       </c>
       <c r="B76" t="n">
         <v>0.05607</v>
@@ -18115,8 +17812,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="s">
-        <v>151</v>
+      <c r="A77" t="n">
+        <v>72</v>
       </c>
       <c r="B77" t="n">
         <v>0.062863</v>
@@ -18348,8 +18045,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="s">
-        <v>152</v>
+      <c r="A78" t="n">
+        <v>73</v>
       </c>
       <c r="B78" t="n">
         <v>0.072532</v>
@@ -18581,8 +18278,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="s">
-        <v>153</v>
+      <c r="A79" t="n">
+        <v>74</v>
       </c>
       <c r="B79" t="n">
         <v>0.072084</v>
@@ -18814,8 +18511,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="s">
-        <v>154</v>
+      <c r="A80" t="n">
+        <v>75</v>
       </c>
       <c r="B80" t="n">
         <v>0.086721</v>
@@ -19047,8 +18744,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="s">
-        <v>155</v>
+      <c r="A81" t="n">
+        <v>76</v>
       </c>
       <c r="B81" t="n">
         <v>0.092739</v>
@@ -19280,8 +18977,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="s">
-        <v>156</v>
+      <c r="A82" t="n">
+        <v>77</v>
       </c>
       <c r="B82" t="n">
         <v>0.102939</v>
@@ -19513,8 +19210,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s">
-        <v>157</v>
+      <c r="A83" t="n">
+        <v>78</v>
       </c>
       <c r="B83" t="n">
         <v>0.110995</v>
@@ -19746,8 +19443,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s">
-        <v>158</v>
+      <c r="A84" t="n">
+        <v>79</v>
       </c>
       <c r="B84" t="n">
         <v>0.12504</v>
@@ -19979,8 +19676,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s">
-        <v>159</v>
+      <c r="A85" t="n">
+        <v>80</v>
       </c>
       <c r="B85" t="n">
         <v>0.135198</v>
@@ -20212,8 +19909,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s">
-        <v>160</v>
+      <c r="A86" t="n">
+        <v>81</v>
       </c>
       <c r="B86" t="n">
         <v>0.139282</v>
@@ -20445,8 +20142,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="s">
-        <v>161</v>
+      <c r="A87" t="n">
+        <v>82</v>
       </c>
       <c r="B87" t="n">
         <v>0.161976</v>
@@ -20678,8 +20375,8 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="s">
-        <v>162</v>
+      <c r="A88" t="n">
+        <v>83</v>
       </c>
       <c r="B88" t="n">
         <v>0.172127</v>
@@ -20911,8 +20608,8 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="s">
-        <v>163</v>
+      <c r="A89" t="n">
+        <v>84</v>
       </c>
       <c r="B89" t="n">
         <v>0.183167</v>
@@ -21144,8 +20841,8 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="s">
-        <v>164</v>
+      <c r="A90" t="n">
+        <v>85</v>
       </c>
       <c r="B90" t="n">
         <v>0.209699</v>
@@ -21377,8 +21074,8 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="s">
-        <v>165</v>
+      <c r="A91" t="n">
+        <v>86</v>
       </c>
       <c r="B91" t="n">
         <v>0.219686</v>
@@ -21610,8 +21307,8 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="s">
-        <v>166</v>
+      <c r="A92" t="n">
+        <v>87</v>
       </c>
       <c r="B92" t="n">
         <v>0.241875</v>
@@ -21843,8 +21540,8 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s">
-        <v>167</v>
+      <c r="A93" t="n">
+        <v>88</v>
       </c>
       <c r="B93" t="n">
         <v>0.256851</v>
@@ -22076,8 +21773,8 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="s">
-        <v>168</v>
+      <c r="A94" t="n">
+        <v>89</v>
       </c>
       <c r="B94" t="n">
         <v>0.277212</v>
@@ -22309,8 +22006,8 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="s">
-        <v>169</v>
+      <c r="A95" t="n">
+        <v>90</v>
       </c>
       <c r="B95" t="n">
         <v>0.305396</v>
@@ -22542,8 +22239,8 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="s">
-        <v>170</v>
+      <c r="A96" t="n">
+        <v>91</v>
       </c>
       <c r="B96" t="n">
         <v>0.335766</v>
@@ -22775,8 +22472,8 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="s">
-        <v>171</v>
+      <c r="A97" t="n">
+        <v>92</v>
       </c>
       <c r="B97" t="n">
         <v>0.283871</v>
@@ -23008,8 +22705,8 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s">
-        <v>172</v>
+      <c r="A98" t="n">
+        <v>93</v>
       </c>
       <c r="B98" t="n">
         <v>0.4</v>
@@ -23241,8 +22938,8 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="s">
-        <v>173</v>
+      <c r="A99" t="n">
+        <v>94</v>
       </c>
       <c r="B99" t="n">
         <v>0.447059</v>
@@ -23474,8 +23171,8 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="s">
-        <v>174</v>
+      <c r="A100" t="n">
+        <v>95</v>
       </c>
       <c r="B100" t="n">
         <v>0.308458</v>
@@ -23707,8 +23404,8 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="s">
-        <v>175</v>
+      <c r="A101" t="n">
+        <v>96</v>
       </c>
       <c r="B101"/>
       <c r="C101"/>
@@ -23830,8 +23527,8 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s">
-        <v>176</v>
+      <c r="A102" t="n">
+        <v>97</v>
       </c>
       <c r="B102"/>
       <c r="C102"/>
@@ -23953,8 +23650,8 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s">
-        <v>177</v>
+      <c r="A103" t="n">
+        <v>98</v>
       </c>
       <c r="B103"/>
       <c r="C103"/>
@@ -24076,8 +23773,8 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="s">
-        <v>178</v>
+      <c r="A104" t="n">
+        <v>99</v>
       </c>
       <c r="B104"/>
       <c r="C104"/>
@@ -24199,8 +23896,8 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="s">
-        <v>179</v>
+      <c r="A105" t="n">
+        <v>100</v>
       </c>
       <c r="B105"/>
       <c r="C105"/>
@@ -24313,7 +24010,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">
@@ -24555,8 +24252,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>79</v>
+      <c r="A5" t="n">
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>0.069991</v>
@@ -24788,8 +24485,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>80</v>
+      <c r="A6" t="n">
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>0.006372</v>
@@ -25021,8 +24718,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>81</v>
+      <c r="A7" t="n">
+        <v>2</v>
       </c>
       <c r="B7" t="n">
         <v>0.004442</v>
@@ -25254,8 +24951,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>82</v>
+      <c r="A8" t="n">
+        <v>3</v>
       </c>
       <c r="B8" t="n">
         <v>0.00331</v>
@@ -25487,8 +25184,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>83</v>
+      <c r="A9" t="n">
+        <v>4</v>
       </c>
       <c r="B9" t="n">
         <v>0.002358</v>
@@ -25720,8 +25417,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>84</v>
+      <c r="A10" t="n">
+        <v>5</v>
       </c>
       <c r="B10" t="n">
         <v>0.001767</v>
@@ -25953,8 +25650,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>85</v>
+      <c r="A11" t="n">
+        <v>6</v>
       </c>
       <c r="B11" t="n">
         <v>0.001243</v>
@@ -26186,8 +25883,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>86</v>
+      <c r="A12" t="n">
+        <v>7</v>
       </c>
       <c r="B12" t="n">
         <v>0.001295</v>
@@ -26419,8 +26116,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>87</v>
+      <c r="A13" t="n">
+        <v>8</v>
       </c>
       <c r="B13" t="n">
         <v>0.001146</v>
@@ -26652,8 +26349,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>88</v>
+      <c r="A14" t="n">
+        <v>9</v>
       </c>
       <c r="B14" t="n">
         <v>0.000865</v>
@@ -26885,8 +26582,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>89</v>
+      <c r="A15" t="n">
+        <v>10</v>
       </c>
       <c r="B15" t="n">
         <v>0.001161</v>
@@ -27118,8 +26815,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>90</v>
+      <c r="A16" t="n">
+        <v>11</v>
       </c>
       <c r="B16" t="n">
         <v>0.00096</v>
@@ -27351,8 +27048,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>91</v>
+      <c r="A17" t="n">
+        <v>12</v>
       </c>
       <c r="B17" t="n">
         <v>0.000921</v>
@@ -27584,8 +27281,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>92</v>
+      <c r="A18" t="n">
+        <v>13</v>
       </c>
       <c r="B18" t="n">
         <v>0.001169</v>
@@ -27817,8 +27514,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>93</v>
+      <c r="A19" t="n">
+        <v>14</v>
       </c>
       <c r="B19" t="n">
         <v>0.001133</v>
@@ -28050,8 +27747,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>94</v>
+      <c r="A20" t="n">
+        <v>15</v>
       </c>
       <c r="B20" t="n">
         <v>0.001293</v>
@@ -28283,8 +27980,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>95</v>
+      <c r="A21" t="n">
+        <v>16</v>
       </c>
       <c r="B21" t="n">
         <v>0.001641</v>
@@ -28516,8 +28213,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>96</v>
+      <c r="A22" t="n">
+        <v>17</v>
       </c>
       <c r="B22" t="n">
         <v>0.001816</v>
@@ -28749,8 +28446,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>97</v>
+      <c r="A23" t="n">
+        <v>18</v>
       </c>
       <c r="B23" t="n">
         <v>0.001668</v>
@@ -28982,8 +28679,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>98</v>
+      <c r="A24" t="n">
+        <v>19</v>
       </c>
       <c r="B24" t="n">
         <v>0.002018</v>
@@ -29215,8 +28912,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>99</v>
+      <c r="A25" t="n">
+        <v>20</v>
       </c>
       <c r="B25" t="n">
         <v>0.002554</v>
@@ -29448,8 +29145,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>100</v>
+      <c r="A26" t="n">
+        <v>21</v>
       </c>
       <c r="B26" t="n">
         <v>0.002803</v>
@@ -29681,8 +29378,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>101</v>
+      <c r="A27" t="n">
+        <v>22</v>
       </c>
       <c r="B27" t="n">
         <v>0.002359</v>
@@ -29914,8 +29611,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>102</v>
+      <c r="A28" t="n">
+        <v>23</v>
       </c>
       <c r="B28" t="n">
         <v>0.002221</v>
@@ -30147,8 +29844,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>103</v>
+      <c r="A29" t="n">
+        <v>24</v>
       </c>
       <c r="B29" t="n">
         <v>0.002659</v>
@@ -30380,8 +30077,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>104</v>
+      <c r="A30" t="n">
+        <v>25</v>
       </c>
       <c r="B30" t="n">
         <v>0.002144</v>
@@ -30613,8 +30310,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>105</v>
+      <c r="A31" t="n">
+        <v>26</v>
       </c>
       <c r="B31" t="n">
         <v>0.00278</v>
@@ -30846,8 +30543,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>106</v>
+      <c r="A32" t="n">
+        <v>27</v>
       </c>
       <c r="B32" t="n">
         <v>0.002528</v>
@@ -31079,8 +30776,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>107</v>
+      <c r="A33" t="n">
+        <v>28</v>
       </c>
       <c r="B33" t="n">
         <v>0.002204</v>
@@ -31312,8 +31009,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>108</v>
+      <c r="A34" t="n">
+        <v>29</v>
       </c>
       <c r="B34" t="n">
         <v>0.002102</v>
@@ -31545,8 +31242,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>109</v>
+      <c r="A35" t="n">
+        <v>30</v>
       </c>
       <c r="B35" t="n">
         <v>0.003083</v>
@@ -31778,8 +31475,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>110</v>
+      <c r="A36" t="n">
+        <v>31</v>
       </c>
       <c r="B36" t="n">
         <v>0.002652</v>
@@ -32011,8 +31708,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>111</v>
+      <c r="A37" t="n">
+        <v>32</v>
       </c>
       <c r="B37" t="n">
         <v>0.003037</v>
@@ -32244,8 +31941,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>112</v>
+      <c r="A38" t="n">
+        <v>33</v>
       </c>
       <c r="B38" t="n">
         <v>0.00276</v>
@@ -32477,8 +32174,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>113</v>
+      <c r="A39" t="n">
+        <v>34</v>
       </c>
       <c r="B39" t="n">
         <v>0.003082</v>
@@ -32710,8 +32407,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
-        <v>114</v>
+      <c r="A40" t="n">
+        <v>35</v>
       </c>
       <c r="B40" t="n">
         <v>0.002907</v>
@@ -32943,8 +32640,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>115</v>
+      <c r="A41" t="n">
+        <v>36</v>
       </c>
       <c r="B41" t="n">
         <v>0.002921</v>
@@ -33176,8 +32873,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>116</v>
+      <c r="A42" t="n">
+        <v>37</v>
       </c>
       <c r="B42" t="n">
         <v>0.003067</v>
@@ -33409,8 +33106,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>117</v>
+      <c r="A43" t="n">
+        <v>38</v>
       </c>
       <c r="B43" t="n">
         <v>0.003574</v>
@@ -33642,8 +33339,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>118</v>
+      <c r="A44" t="n">
+        <v>39</v>
       </c>
       <c r="B44" t="n">
         <v>0.003543</v>
@@ -33875,8 +33572,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s">
-        <v>119</v>
+      <c r="A45" t="n">
+        <v>40</v>
       </c>
       <c r="B45" t="n">
         <v>0.004066</v>
@@ -34108,8 +33805,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
-        <v>120</v>
+      <c r="A46" t="n">
+        <v>41</v>
       </c>
       <c r="B46" t="n">
         <v>0.003936</v>
@@ -34341,8 +34038,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s">
-        <v>121</v>
+      <c r="A47" t="n">
+        <v>42</v>
       </c>
       <c r="B47" t="n">
         <v>0.003941</v>
@@ -34574,8 +34271,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>122</v>
+      <c r="A48" t="n">
+        <v>43</v>
       </c>
       <c r="B48" t="n">
         <v>0.003872</v>
@@ -34807,8 +34504,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s">
-        <v>123</v>
+      <c r="A49" t="n">
+        <v>44</v>
       </c>
       <c r="B49" t="n">
         <v>0.004598</v>
@@ -35040,8 +34737,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>124</v>
+      <c r="A50" t="n">
+        <v>45</v>
       </c>
       <c r="B50" t="n">
         <v>0.004493</v>
@@ -35273,8 +34970,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s">
-        <v>125</v>
+      <c r="A51" t="n">
+        <v>46</v>
       </c>
       <c r="B51" t="n">
         <v>0.004952</v>
@@ -35506,8 +35203,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>126</v>
+      <c r="A52" t="n">
+        <v>47</v>
       </c>
       <c r="B52" t="n">
         <v>0.005277</v>
@@ -35739,8 +35436,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s">
-        <v>127</v>
+      <c r="A53" t="n">
+        <v>48</v>
       </c>
       <c r="B53" t="n">
         <v>0.006303</v>
@@ -35972,8 +35669,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s">
-        <v>128</v>
+      <c r="A54" t="n">
+        <v>49</v>
       </c>
       <c r="B54" t="n">
         <v>0.006407</v>
@@ -36205,8 +35902,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s">
-        <v>129</v>
+      <c r="A55" t="n">
+        <v>50</v>
       </c>
       <c r="B55" t="n">
         <v>0.006817</v>
@@ -36438,8 +36135,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s">
-        <v>130</v>
+      <c r="A56" t="n">
+        <v>51</v>
       </c>
       <c r="B56" t="n">
         <v>0.007016</v>
@@ -36671,8 +36368,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="s">
-        <v>131</v>
+      <c r="A57" t="n">
+        <v>52</v>
       </c>
       <c r="B57" t="n">
         <v>0.007325</v>
@@ -36904,8 +36601,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s">
-        <v>132</v>
+      <c r="A58" t="n">
+        <v>53</v>
       </c>
       <c r="B58" t="n">
         <v>0.006968</v>
@@ -37137,8 +36834,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s">
-        <v>133</v>
+      <c r="A59" t="n">
+        <v>54</v>
       </c>
       <c r="B59" t="n">
         <v>0.008224</v>
@@ -37370,8 +37067,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s">
-        <v>134</v>
+      <c r="A60" t="n">
+        <v>55</v>
       </c>
       <c r="B60" t="n">
         <v>0.009288</v>
@@ -37603,8 +37300,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s">
-        <v>135</v>
+      <c r="A61" t="n">
+        <v>56</v>
       </c>
       <c r="B61" t="n">
         <v>0.009614</v>
@@ -37836,8 +37533,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
-        <v>136</v>
+      <c r="A62" t="n">
+        <v>57</v>
       </c>
       <c r="B62" t="n">
         <v>0.011798</v>
@@ -38069,8 +37766,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s">
-        <v>137</v>
+      <c r="A63" t="n">
+        <v>58</v>
       </c>
       <c r="B63" t="n">
         <v>0.011307</v>
@@ -38302,8 +37999,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s">
-        <v>138</v>
+      <c r="A64" t="n">
+        <v>59</v>
       </c>
       <c r="B64" t="n">
         <v>0.013849</v>
@@ -38535,8 +38232,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s">
-        <v>139</v>
+      <c r="A65" t="n">
+        <v>60</v>
       </c>
       <c r="B65" t="n">
         <v>0.013245</v>
@@ -38768,8 +38465,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s">
-        <v>140</v>
+      <c r="A66" t="n">
+        <v>61</v>
       </c>
       <c r="B66" t="n">
         <v>0.016543</v>
@@ -39001,8 +38698,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s">
-        <v>141</v>
+      <c r="A67" t="n">
+        <v>62</v>
       </c>
       <c r="B67" t="n">
         <v>0.01754</v>
@@ -39234,8 +38931,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s">
-        <v>142</v>
+      <c r="A68" t="n">
+        <v>63</v>
       </c>
       <c r="B68" t="n">
         <v>0.020477</v>
@@ -39467,8 +39164,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="s">
-        <v>143</v>
+      <c r="A69" t="n">
+        <v>64</v>
       </c>
       <c r="B69" t="n">
         <v>0.021504</v>
@@ -39700,8 +39397,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="s">
-        <v>144</v>
+      <c r="A70" t="n">
+        <v>65</v>
       </c>
       <c r="B70" t="n">
         <v>0.02436</v>
@@ -39933,8 +39630,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="s">
-        <v>145</v>
+      <c r="A71" t="n">
+        <v>66</v>
       </c>
       <c r="B71" t="n">
         <v>0.027273</v>
@@ -40166,8 +39863,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="s">
-        <v>146</v>
+      <c r="A72" t="n">
+        <v>67</v>
       </c>
       <c r="B72" t="n">
         <v>0.028473</v>
@@ -40399,8 +40096,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s">
-        <v>147</v>
+      <c r="A73" t="n">
+        <v>68</v>
       </c>
       <c r="B73" t="n">
         <v>0.0322</v>
@@ -40632,8 +40329,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s">
-        <v>148</v>
+      <c r="A74" t="n">
+        <v>69</v>
       </c>
       <c r="B74" t="n">
         <v>0.036993</v>
@@ -40865,8 +40562,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="s">
-        <v>149</v>
+      <c r="A75" t="n">
+        <v>70</v>
       </c>
       <c r="B75" t="n">
         <v>0.042184</v>
@@ -41098,8 +40795,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="s">
-        <v>150</v>
+      <c r="A76" t="n">
+        <v>71</v>
       </c>
       <c r="B76" t="n">
         <v>0.045327</v>
@@ -41331,8 +41028,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="s">
-        <v>151</v>
+      <c r="A77" t="n">
+        <v>72</v>
       </c>
       <c r="B77" t="n">
         <v>0.050426</v>
@@ -41564,8 +41261,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="s">
-        <v>152</v>
+      <c r="A78" t="n">
+        <v>73</v>
       </c>
       <c r="B78" t="n">
         <v>0.054274</v>
@@ -41797,8 +41494,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="s">
-        <v>153</v>
+      <c r="A79" t="n">
+        <v>74</v>
       </c>
       <c r="B79" t="n">
         <v>0.061368</v>
@@ -42030,8 +41727,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="s">
-        <v>154</v>
+      <c r="A80" t="n">
+        <v>75</v>
       </c>
       <c r="B80" t="n">
         <v>0.071952</v>
@@ -42263,8 +41960,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="s">
-        <v>155</v>
+      <c r="A81" t="n">
+        <v>76</v>
       </c>
       <c r="B81" t="n">
         <v>0.077303</v>
@@ -42496,8 +42193,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="s">
-        <v>156</v>
+      <c r="A82" t="n">
+        <v>77</v>
       </c>
       <c r="B82" t="n">
         <v>0.084891</v>
@@ -42729,8 +42426,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s">
-        <v>157</v>
+      <c r="A83" t="n">
+        <v>78</v>
       </c>
       <c r="B83" t="n">
         <v>0.094687</v>
@@ -42962,8 +42659,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s">
-        <v>158</v>
+      <c r="A84" t="n">
+        <v>79</v>
       </c>
       <c r="B84" t="n">
         <v>0.105782</v>
@@ -43195,8 +42892,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s">
-        <v>159</v>
+      <c r="A85" t="n">
+        <v>80</v>
       </c>
       <c r="B85" t="n">
         <v>0.118683</v>
@@ -43428,8 +43125,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s">
-        <v>160</v>
+      <c r="A86" t="n">
+        <v>81</v>
       </c>
       <c r="B86" t="n">
         <v>0.127842</v>
@@ -43661,8 +43358,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="s">
-        <v>161</v>
+      <c r="A87" t="n">
+        <v>82</v>
       </c>
       <c r="B87" t="n">
         <v>0.129022</v>
@@ -43894,8 +43591,8 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="s">
-        <v>162</v>
+      <c r="A88" t="n">
+        <v>83</v>
       </c>
       <c r="B88" t="n">
         <v>0.153819</v>
@@ -44127,8 +43824,8 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="s">
-        <v>163</v>
+      <c r="A89" t="n">
+        <v>84</v>
       </c>
       <c r="B89" t="n">
         <v>0.169676</v>
@@ -44360,8 +44057,8 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="s">
-        <v>164</v>
+      <c r="A90" t="n">
+        <v>85</v>
       </c>
       <c r="B90" t="n">
         <v>0.168753</v>
@@ -44593,8 +44290,8 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="s">
-        <v>165</v>
+      <c r="A91" t="n">
+        <v>86</v>
       </c>
       <c r="B91" t="n">
         <v>0.189458</v>
@@ -44826,8 +44523,8 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="s">
-        <v>166</v>
+      <c r="A92" t="n">
+        <v>87</v>
       </c>
       <c r="B92" t="n">
         <v>0.213667</v>
@@ -45059,8 +44756,8 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s">
-        <v>167</v>
+      <c r="A93" t="n">
+        <v>88</v>
       </c>
       <c r="B93" t="n">
         <v>0.224173</v>
@@ -45292,8 +44989,8 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="s">
-        <v>168</v>
+      <c r="A94" t="n">
+        <v>89</v>
       </c>
       <c r="B94" t="n">
         <v>0.261029</v>
@@ -45525,8 +45222,8 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="s">
-        <v>169</v>
+      <c r="A95" t="n">
+        <v>90</v>
       </c>
       <c r="B95" t="n">
         <v>0.2587</v>
@@ -45758,8 +45455,8 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="s">
-        <v>170</v>
+      <c r="A96" t="n">
+        <v>91</v>
       </c>
       <c r="B96" t="n">
         <v>0.26703</v>
@@ -45991,8 +45688,8 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="s">
-        <v>171</v>
+      <c r="A97" t="n">
+        <v>92</v>
       </c>
       <c r="B97" t="n">
         <v>0.25097</v>
@@ -46224,8 +45921,8 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s">
-        <v>172</v>
+      <c r="A98" t="n">
+        <v>93</v>
       </c>
       <c r="B98" t="n">
         <v>0.354379</v>
@@ -46457,8 +46154,8 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="s">
-        <v>173</v>
+      <c r="A99" t="n">
+        <v>94</v>
       </c>
       <c r="B99" t="n">
         <v>0.240964</v>
@@ -46690,8 +46387,8 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="s">
-        <v>174</v>
+      <c r="A100" t="n">
+        <v>95</v>
       </c>
       <c r="B100" t="n">
         <v>0.332553</v>
@@ -46923,8 +46620,8 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="s">
-        <v>175</v>
+      <c r="A101" t="n">
+        <v>96</v>
       </c>
       <c r="B101"/>
       <c r="C101"/>
@@ -47046,8 +46743,8 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s">
-        <v>176</v>
+      <c r="A102" t="n">
+        <v>97</v>
       </c>
       <c r="B102"/>
       <c r="C102"/>
@@ -47169,8 +46866,8 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s">
-        <v>177</v>
+      <c r="A103" t="n">
+        <v>98</v>
       </c>
       <c r="B103"/>
       <c r="C103"/>
@@ -47292,8 +46989,8 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="s">
-        <v>178</v>
+      <c r="A104" t="n">
+        <v>99</v>
       </c>
       <c r="B104"/>
       <c r="C104"/>
@@ -47415,8 +47112,8 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="s">
-        <v>179</v>
+      <c r="A105" t="n">
+        <v>100</v>
       </c>
       <c r="B105"/>
       <c r="C105"/>
@@ -47529,7 +47226,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2">
@@ -47606,8 +47303,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
-        <v>79</v>
+      <c r="A5" t="n">
+        <v>0</v>
       </c>
       <c r="B5" t="n">
         <v>0.00405617418589523</v>
@@ -47674,8 +47371,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
-        <v>80</v>
+      <c r="A6" t="n">
+        <v>1</v>
       </c>
       <c r="B6" t="n">
         <v>0.000410425447660334</v>
@@ -47742,8 +47439,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>81</v>
+      <c r="A7" t="n">
+        <v>2</v>
       </c>
       <c r="B7" t="n">
         <v>0.000125292675860017</v>
@@ -47810,8 +47507,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s">
-        <v>82</v>
+      <c r="A8" t="n">
+        <v>3</v>
       </c>
       <c r="B8" t="n">
         <v>0.00012292619664811</v>
@@ -47878,8 +47575,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s">
-        <v>83</v>
+      <c r="A9" t="n">
+        <v>4</v>
       </c>
       <c r="B9" t="n">
         <v>0.000131026083124138</v>
@@ -47946,8 +47643,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="s">
-        <v>84</v>
+      <c r="A10" t="n">
+        <v>5</v>
       </c>
       <c r="B10" t="n">
         <v>0.000123662026061772</v>
@@ -48014,8 +47711,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="s">
-        <v>85</v>
+      <c r="A11" t="n">
+        <v>6</v>
       </c>
       <c r="B11" t="n">
         <v>0.0000888776557407328</v>
@@ -48082,8 +47779,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="s">
-        <v>86</v>
+      <c r="A12" t="n">
+        <v>7</v>
       </c>
       <c r="B12" t="n">
         <v>0.000065594291110197</v>
@@ -48150,8 +47847,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="s">
-        <v>87</v>
+      <c r="A13" t="n">
+        <v>8</v>
       </c>
       <c r="B13" t="n">
         <v>0.000115840687461825</v>
@@ -48218,8 +47915,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="s">
-        <v>88</v>
+      <c r="A14" t="n">
+        <v>9</v>
       </c>
       <c r="B14" t="n">
         <v>0.000113472543512852</v>
@@ -48286,8 +47983,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="s">
-        <v>89</v>
+      <c r="A15" t="n">
+        <v>10</v>
       </c>
       <c r="B15" t="n">
         <v>0.000132776353552789</v>
@@ -48354,8 +48051,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="s">
-        <v>90</v>
+      <c r="A16" t="n">
+        <v>11</v>
       </c>
       <c r="B16" t="n">
         <v>0.0000719411521375515</v>
@@ -48422,8 +48119,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="s">
-        <v>91</v>
+      <c r="A17" t="n">
+        <v>12</v>
       </c>
       <c r="B17" t="n">
         <v>0.000135912535056286</v>
@@ -48490,8 +48187,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="s">
-        <v>92</v>
+      <c r="A18" t="n">
+        <v>13</v>
       </c>
       <c r="B18" t="n">
         <v>0.000114974065509087</v>
@@ -48558,8 +48255,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="s">
-        <v>93</v>
+      <c r="A19" t="n">
+        <v>14</v>
       </c>
       <c r="B19" t="n">
         <v>0.000157586613542468</v>
@@ -48626,8 +48323,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="s">
-        <v>94</v>
+      <c r="A20" t="n">
+        <v>15</v>
       </c>
       <c r="B20" t="n">
         <v>0.000276768356860861</v>
@@ -48694,8 +48391,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="s">
-        <v>95</v>
+      <c r="A21" t="n">
+        <v>16</v>
       </c>
       <c r="B21" t="n">
         <v>0.000413100584696212</v>
@@ -48762,8 +48459,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="s">
-        <v>96</v>
+      <c r="A22" t="n">
+        <v>17</v>
       </c>
       <c r="B22" t="n">
         <v>0.000551319526073253</v>
@@ -48830,8 +48527,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="s">
-        <v>97</v>
+      <c r="A23" t="n">
+        <v>18</v>
       </c>
       <c r="B23" t="n">
         <v>0.000649775930443034</v>
@@ -48898,8 +48595,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="s">
-        <v>98</v>
+      <c r="A24" t="n">
+        <v>19</v>
       </c>
       <c r="B24" t="n">
         <v>0.000674796113375819</v>
@@ -48966,8 +48663,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="s">
-        <v>99</v>
+      <c r="A25" t="n">
+        <v>20</v>
       </c>
       <c r="B25" t="n">
         <v>0.000599521856748675</v>
@@ -49034,8 +48731,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="s">
-        <v>100</v>
+      <c r="A26" t="n">
+        <v>21</v>
       </c>
       <c r="B26" t="n">
         <v>0.000634450147336177</v>
@@ -49102,8 +48799,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="s">
-        <v>101</v>
+      <c r="A27" t="n">
+        <v>22</v>
       </c>
       <c r="B27" t="n">
         <v>0.000673377128745822</v>
@@ -49170,8 +48867,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="s">
-        <v>102</v>
+      <c r="A28" t="n">
+        <v>23</v>
       </c>
       <c r="B28" t="n">
         <v>0.00063205381938272</v>
@@ -49238,8 +48935,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="s">
-        <v>103</v>
+      <c r="A29" t="n">
+        <v>24</v>
       </c>
       <c r="B29" t="n">
         <v>0.000580903331084533</v>
@@ -49306,8 +49003,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="s">
-        <v>104</v>
+      <c r="A30" t="n">
+        <v>25</v>
       </c>
       <c r="B30" t="n">
         <v>0.000697135112848746</v>
@@ -49374,8 +49071,8 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>105</v>
+      <c r="A31" t="n">
+        <v>26</v>
       </c>
       <c r="B31" t="n">
         <v>0.000550344653339154</v>
@@ -49442,8 +49139,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>106</v>
+      <c r="A32" t="n">
+        <v>27</v>
       </c>
       <c r="B32" t="n">
         <v>0.000674180775402847</v>
@@ -49510,8 +49207,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>107</v>
+      <c r="A33" t="n">
+        <v>28</v>
       </c>
       <c r="B33" t="n">
         <v>0.000651211252930451</v>
@@ -49578,8 +49275,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>108</v>
+      <c r="A34" t="n">
+        <v>29</v>
       </c>
       <c r="B34" t="n">
         <v>0.000570958932217584</v>
@@ -49646,8 +49343,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>109</v>
+      <c r="A35" t="n">
+        <v>30</v>
       </c>
       <c r="B35" t="n">
         <v>0.000587742010644428</v>
@@ -49714,8 +49411,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>110</v>
+      <c r="A36" t="n">
+        <v>31</v>
       </c>
       <c r="B36" t="n">
         <v>0.000509921720945338</v>
@@ -49782,8 +49479,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>111</v>
+      <c r="A37" t="n">
+        <v>32</v>
       </c>
       <c r="B37" t="n">
         <v>0.000599526143759452</v>
@@ -49850,8 +49547,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>112</v>
+      <c r="A38" t="n">
+        <v>33</v>
       </c>
       <c r="B38" t="n">
         <v>0.000750815053477349</v>
@@ -49918,8 +49615,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>113</v>
+      <c r="A39" t="n">
+        <v>34</v>
       </c>
       <c r="B39" t="n">
         <v>0.000792070729775437</v>
@@ -49986,8 +49683,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
-        <v>114</v>
+      <c r="A40" t="n">
+        <v>35</v>
       </c>
       <c r="B40" t="n">
         <v>0.000872188621513033</v>
@@ -50054,8 +49751,8 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>115</v>
+      <c r="A41" t="n">
+        <v>36</v>
       </c>
       <c r="B41" t="n">
         <v>0.00071088552343834</v>
@@ -50122,8 +49819,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>116</v>
+      <c r="A42" t="n">
+        <v>37</v>
       </c>
       <c r="B42" t="n">
         <v>0.000884912588752552</v>
@@ -50190,8 +49887,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>117</v>
+      <c r="A43" t="n">
+        <v>38</v>
       </c>
       <c r="B43" t="n">
         <v>0.00121566319143027</v>
@@ -50258,8 +49955,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>118</v>
+      <c r="A44" t="n">
+        <v>39</v>
       </c>
       <c r="B44" t="n">
         <v>0.00124273317044401</v>
@@ -50326,8 +50023,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s">
-        <v>119</v>
+      <c r="A45" t="n">
+        <v>40</v>
       </c>
       <c r="B45" t="n">
         <v>0.00150303483588873</v>
@@ -50394,8 +50091,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
-        <v>120</v>
+      <c r="A46" t="n">
+        <v>41</v>
       </c>
       <c r="B46" t="n">
         <v>0.00150348522461116</v>
@@ -50462,8 +50159,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s">
-        <v>121</v>
+      <c r="A47" t="n">
+        <v>42</v>
       </c>
       <c r="B47" t="n">
         <v>0.0015279747999332</v>
@@ -50530,8 +50227,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>122</v>
+      <c r="A48" t="n">
+        <v>43</v>
       </c>
       <c r="B48" t="n">
         <v>0.001726078874213</v>
@@ -50598,8 +50295,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s">
-        <v>123</v>
+      <c r="A49" t="n">
+        <v>44</v>
       </c>
       <c r="B49" t="n">
         <v>0.00209397970529709</v>
@@ -50666,8 +50363,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>124</v>
+      <c r="A50" t="n">
+        <v>45</v>
       </c>
       <c r="B50" t="n">
         <v>0.00206858494284588</v>
@@ -50734,8 +50431,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s">
-        <v>125</v>
+      <c r="A51" t="n">
+        <v>46</v>
       </c>
       <c r="B51" t="n">
         <v>0.00231683856055517</v>
@@ -50802,8 +50499,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="s">
-        <v>126</v>
+      <c r="A52" t="n">
+        <v>47</v>
       </c>
       <c r="B52" t="n">
         <v>0.00284365237970633</v>
@@ -50870,8 +50567,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="s">
-        <v>127</v>
+      <c r="A53" t="n">
+        <v>48</v>
       </c>
       <c r="B53" t="n">
         <v>0.00293070662325236</v>
@@ -50938,8 +50635,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="s">
-        <v>128</v>
+      <c r="A54" t="n">
+        <v>49</v>
       </c>
       <c r="B54" t="n">
         <v>0.00302376443994305</v>
@@ -51006,8 +50703,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="s">
-        <v>129</v>
+      <c r="A55" t="n">
+        <v>50</v>
       </c>
       <c r="B55" t="n">
         <v>0.00345248864793046</v>
@@ -51074,8 +50771,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="s">
-        <v>130</v>
+      <c r="A56" t="n">
+        <v>51</v>
       </c>
       <c r="B56" t="n">
         <v>0.00406411882226701</v>
@@ -51142,8 +50839,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="s">
-        <v>131</v>
+      <c r="A57" t="n">
+        <v>52</v>
       </c>
       <c r="B57" t="n">
         <v>0.0044328945680854</v>
@@ -51210,8 +50907,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="s">
-        <v>132</v>
+      <c r="A58" t="n">
+        <v>53</v>
       </c>
       <c r="B58" t="n">
         <v>0.00489924609501619</v>
@@ -51278,8 +50975,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="s">
-        <v>133</v>
+      <c r="A59" t="n">
+        <v>54</v>
       </c>
       <c r="B59" t="n">
         <v>0.005270852752057</v>
@@ -51346,8 +51043,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s">
-        <v>134</v>
+      <c r="A60" t="n">
+        <v>55</v>
       </c>
       <c r="B60" t="n">
         <v>0.00552551469755238</v>
@@ -51414,8 +51111,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="s">
-        <v>135</v>
+      <c r="A61" t="n">
+        <v>56</v>
       </c>
       <c r="B61" t="n">
         <v>0.00613136178338057</v>
@@ -51482,8 +51179,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="s">
-        <v>136</v>
+      <c r="A62" t="n">
+        <v>57</v>
       </c>
       <c r="B62" t="n">
         <v>0.00649076726572019</v>
@@ -51550,8 +51247,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="s">
-        <v>137</v>
+      <c r="A63" t="n">
+        <v>58</v>
       </c>
       <c r="B63" t="n">
         <v>0.00741433046171413</v>
@@ -51618,8 +51315,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s">
-        <v>138</v>
+      <c r="A64" t="n">
+        <v>59</v>
       </c>
       <c r="B64" t="n">
         <v>0.00762832962811893</v>
@@ -51686,8 +51383,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s">
-        <v>139</v>
+      <c r="A65" t="n">
+        <v>60</v>
       </c>
       <c r="B65" t="n">
         <v>0.00710684700290937</v>
@@ -51754,8 +51451,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s">
-        <v>140</v>
+      <c r="A66" t="n">
+        <v>61</v>
       </c>
       <c r="B66" t="n">
         <v>0.00860869575257389</v>
@@ -51822,8 +51519,8 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s">
-        <v>141</v>
+      <c r="A67" t="n">
+        <v>62</v>
       </c>
       <c r="B67" t="n">
         <v>0.00899045901625132</v>
@@ -51890,8 +51587,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="s">
-        <v>142</v>
+      <c r="A68" t="n">
+        <v>63</v>
       </c>
       <c r="B68" t="n">
         <v>0.00964128358982136</v>
@@ -51958,8 +51655,8 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="s">
-        <v>143</v>
+      <c r="A69" t="n">
+        <v>64</v>
       </c>
       <c r="B69" t="n">
         <v>0.0112298048909685</v>
@@ -52026,8 +51723,8 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="s">
-        <v>144</v>
+      <c r="A70" t="n">
+        <v>65</v>
       </c>
       <c r="B70" t="n">
         <v>0.0123107308661134</v>
@@ -52094,8 +51791,8 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="s">
-        <v>145</v>
+      <c r="A71" t="n">
+        <v>66</v>
       </c>
       <c r="B71" t="n">
         <v>0.0134965180433866</v>
@@ -52162,8 +51859,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="s">
-        <v>146</v>
+      <c r="A72" t="n">
+        <v>67</v>
       </c>
       <c r="B72" t="n">
         <v>0.0147917072352502</v>
@@ -52230,8 +51927,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s">
-        <v>147</v>
+      <c r="A73" t="n">
+        <v>68</v>
       </c>
       <c r="B73" t="n">
         <v>0.0171136395325073</v>
@@ -52298,8 +51995,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s">
-        <v>148</v>
+      <c r="A74" t="n">
+        <v>69</v>
       </c>
       <c r="B74" t="n">
         <v>0.0167537526933093</v>
@@ -52366,8 +52063,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="s">
-        <v>149</v>
+      <c r="A75" t="n">
+        <v>70</v>
       </c>
       <c r="B75" t="n">
         <v>0.0211071618617466</v>
@@ -52434,8 +52131,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="s">
-        <v>150</v>
+      <c r="A76" t="n">
+        <v>71</v>
       </c>
       <c r="B76" t="n">
         <v>0.0217392907445781</v>
@@ -52502,8 +52199,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="s">
-        <v>151</v>
+      <c r="A77" t="n">
+        <v>72</v>
       </c>
       <c r="B77" t="n">
         <v>0.0243776515746706</v>
@@ -52570,8 +52267,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="s">
-        <v>152</v>
+      <c r="A78" t="n">
+        <v>73</v>
       </c>
       <c r="B78" t="n">
         <v>0.0273584814575227</v>
@@ -52638,8 +52335,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="s">
-        <v>153</v>
+      <c r="A79" t="n">
+        <v>74</v>
       </c>
       <c r="B79" t="n">
         <v>0.029406810251474</v>
@@ -52706,8 +52403,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="s">
-        <v>154</v>
+      <c r="A80" t="n">
+        <v>75</v>
       </c>
       <c r="B80" t="n">
         <v>0.0322274571391179</v>
@@ -52774,8 +52471,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="s">
-        <v>155</v>
+      <c r="A81" t="n">
+        <v>76</v>
       </c>
       <c r="B81" t="n">
         <v>0.0370451565401909</v>
@@ -52842,8 +52539,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="s">
-        <v>156</v>
+      <c r="A82" t="n">
+        <v>77</v>
       </c>
       <c r="B82" t="n">
         <v>0.0408670908470684</v>
@@ -52910,8 +52607,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s">
-        <v>157</v>
+      <c r="A83" t="n">
+        <v>78</v>
       </c>
       <c r="B83" t="n">
         <v>0.0444657808157639</v>
@@ -52978,8 +52675,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s">
-        <v>158</v>
+      <c r="A84" t="n">
+        <v>79</v>
       </c>
       <c r="B84" t="n">
         <v>0.0510997222544477</v>
@@ -53046,8 +52743,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s">
-        <v>159</v>
+      <c r="A85" t="n">
+        <v>80</v>
       </c>
       <c r="B85" t="n">
         <v>0.0563087390118433</v>
@@ -53114,8 +52811,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s">
-        <v>160</v>
+      <c r="A86" t="n">
+        <v>81</v>
       </c>
       <c r="B86" t="n">
         <v>0.0630344347899958</v>
@@ -53182,8 +52879,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="s">
-        <v>161</v>
+      <c r="A87" t="n">
+        <v>82</v>
       </c>
       <c r="B87" t="n">
         <v>0.0703001482970353</v>
@@ -53250,8 +52947,8 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="s">
-        <v>162</v>
+      <c r="A88" t="n">
+        <v>83</v>
       </c>
       <c r="B88" t="n">
         <v>0.0830402263998383</v>
@@ -53318,8 +53015,8 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="s">
-        <v>163</v>
+      <c r="A89" t="n">
+        <v>84</v>
       </c>
       <c r="B89" t="n">
         <v>0.0880088603149734</v>
@@ -53386,8 +53083,8 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="s">
-        <v>164</v>
+      <c r="A90" t="n">
+        <v>85</v>
       </c>
       <c r="B90" t="n">
         <v>0.101129746677948</v>
@@ -53454,8 +53151,8 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="s">
-        <v>165</v>
+      <c r="A91" t="n">
+        <v>86</v>
       </c>
       <c r="B91" t="n">
         <v>0.114979483678698</v>
@@ -53522,8 +53219,8 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="s">
-        <v>166</v>
+      <c r="A92" t="n">
+        <v>87</v>
       </c>
       <c r="B92" t="n">
         <v>0.127683839638893</v>
@@ -53590,8 +53287,8 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s">
-        <v>167</v>
+      <c r="A93" t="n">
+        <v>88</v>
       </c>
       <c r="B93" t="n">
         <v>0.140937488215404</v>
@@ -53658,8 +53355,8 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="s">
-        <v>168</v>
+      <c r="A94" t="n">
+        <v>89</v>
       </c>
       <c r="B94" t="n">
         <v>0.163222136466284</v>
@@ -53726,8 +53423,8 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="s">
-        <v>169</v>
+      <c r="A95" t="n">
+        <v>90</v>
       </c>
       <c r="B95" t="n">
         <v>0.173006024638072</v>
@@ -53794,8 +53491,8 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="s">
-        <v>170</v>
+      <c r="A96" t="n">
+        <v>91</v>
       </c>
       <c r="B96" t="n">
         <v>0.198981590285938</v>
@@ -53862,8 +53559,8 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="s">
-        <v>171</v>
+      <c r="A97" t="n">
+        <v>92</v>
       </c>
       <c r="B97" t="n">
         <v>0.215428554775158</v>
@@ -53930,8 +53627,8 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="s">
-        <v>172</v>
+      <c r="A98" t="n">
+        <v>93</v>
       </c>
       <c r="B98" t="n">
         <v>0.242012826837691</v>
@@ -53998,8 +53695,8 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="s">
-        <v>173</v>
+      <c r="A99" t="n">
+        <v>94</v>
       </c>
       <c r="B99" t="n">
         <v>0.258408258408258</v>
@@ -54066,8 +53763,8 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="s">
-        <v>174</v>
+      <c r="A100" t="n">
+        <v>95</v>
       </c>
       <c r="B100" t="n">
         <v>0.285075202468184</v>
@@ -54134,8 +53831,8 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="s">
-        <v>175</v>
+      <c r="A101" t="n">
+        <v>96</v>
       </c>
       <c r="B101" t="n">
         <v>0.305273949196947</v>
@@ -54202,8 +53899,8 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s">
-        <v>176</v>
+      <c r="A102" t="n">
+        <v>97</v>
       </c>
       <c r="B102" t="n">
         <v>0.30940791220462</v>
@@ -54270,8 +53967,8 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s">
-        <v>177</v>
+      <c r="A103" t="n">
+        <v>98</v>
       </c>
       <c r="B103" t="n">
         <v>0.357548083575481</v>
@@ -54338,8 +54035,8 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="s">
-        <v>178</v>
+      <c r="A104" t="n">
+        <v>99</v>
       </c>
       <c r="B104" t="n">
         <v>0.367473167182099</v>
@@ -54406,8 +54103,8 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="s">
-        <v>179</v>
+      <c r="A105" t="n">
+        <v>100</v>
       </c>
       <c r="B105"/>
       <c r="C105"/>

</xml_diff>